<commit_message>
fixed results for mitigation
</commit_message>
<xml_diff>
--- a/Results/Mitigation_direct/results_df_age_direct.xlsx
+++ b/Results/Mitigation_direct/results_df_age_direct.xlsx
@@ -553,16 +553,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>335</v>
+        <v>69.08</v>
       </c>
       <c r="D2" t="n">
-        <v>73</v>
+        <v>7.69</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-68</v>
+        <v>12.62</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -577,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>5</v>
+        <v>0.77</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>6</v>
+        <v>0.92</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -607,10 +607,10 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="V2" t="n">
-        <v>8</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="3">
@@ -621,16 +621,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>356</v>
+        <v>76</v>
       </c>
       <c r="D3" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>-220</v>
+        <v>30</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -689,16 +689,16 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>75.91</v>
       </c>
       <c r="D4" t="n">
-        <v>548</v>
+        <v>33.76</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1986</v>
+        <v>61.31</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -713,25 +713,25 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>0.73</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>0.18</v>
       </c>
       <c r="N4" t="n">
-        <v>2</v>
+        <v>0.36</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>1</v>
+        <v>0.18</v>
       </c>
       <c r="Q4" t="n">
-        <v>10</v>
+        <v>1.82</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>17</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="5">
@@ -757,19 +757,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>82.75</v>
       </c>
       <c r="D5" t="n">
-        <v>185</v>
+        <v>66.75</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>444</v>
+        <v>32.75</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -781,16 +781,16 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
@@ -805,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>11</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="6">
@@ -825,19 +825,19 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>402</v>
+        <v>57.76</v>
       </c>
       <c r="D6" t="n">
-        <v>856</v>
+        <v>56.71</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>404</v>
+        <v>14.08</v>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>0.26</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>0.13</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -858,16 +858,16 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>3</v>
+        <v>0.39</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>2</v>
+        <v>0.26</v>
       </c>
       <c r="Q6" t="n">
-        <v>4</v>
+        <v>0.53</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -879,10 +879,10 @@
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>1</v>
+        <v>0.13</v>
       </c>
       <c r="V6" t="n">
-        <v>5</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="7">
@@ -893,16 +893,16 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>253</v>
+        <v>47.64</v>
       </c>
       <c r="D7" t="n">
-        <v>440</v>
+        <v>18.49</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>850</v>
+        <v>21.81</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>8</v>
+        <v>0.51</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -926,16 +926,16 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>28</v>
+        <v>1.79</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>5</v>
+        <v>0.32</v>
       </c>
       <c r="Q7" t="n">
-        <v>8</v>
+        <v>0.51</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -961,16 +961,16 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>189</v>
+        <v>52.96</v>
       </c>
       <c r="D8" t="n">
-        <v>264</v>
+        <v>31.48</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>171</v>
+        <v>44.07</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -982,10 +982,10 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>14</v>
+        <v>5.19</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -994,16 +994,16 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>2</v>
+        <v>0.74</v>
       </c>
       <c r="Q8" t="n">
-        <v>2</v>
+        <v>0.74</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -1018,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>4</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="9">
@@ -1029,25 +1029,25 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>403</v>
+        <v>57.27</v>
       </c>
       <c r="D9" t="n">
-        <v>537</v>
+        <v>12.1</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-117</v>
+        <v>35.41</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -1068,13 +1068,13 @@
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>6</v>
+        <v>0.21</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -1083,10 +1083,10 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>2</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="V9" t="n">
-        <v>8</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="10">
@@ -1097,46 +1097,46 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>134</v>
+        <v>61.56</v>
       </c>
       <c r="D10" t="n">
-        <v>175</v>
+        <v>14.21</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>485</v>
+        <v>29.21</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>0.16</v>
       </c>
       <c r="H10" t="n">
-        <v>28</v>
+        <v>2.25</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>6</v>
+        <v>0.48</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>9</v>
+        <v>0.72</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>4</v>
+        <v>0.32</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>7</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -1165,31 +1165,31 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>66</v>
+        <v>41.48</v>
       </c>
       <c r="D11" t="n">
-        <v>342</v>
+        <v>58.89</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>823</v>
+        <v>23.33</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>11</v>
+        <v>4.07</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>16</v>
+        <v>5.93</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>4</v>
+        <v>1.48</v>
       </c>
       <c r="R11" t="n">
         <v>0</v>
@@ -1216,13 +1216,13 @@
         <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>43</v>
+        <v>15.93</v>
       </c>
       <c r="U11" t="n">
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>3</v>
+        <v>1.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>